<commit_message>
add 3rd chinese words
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdgandzxx\learngit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F07D5AE-9EED-40CD-A340-1D7EBC7AF2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF40C5E3-B395-4616-9D8D-1DEEE82078C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="240" windowWidth="26115" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="960" windowWidth="26115" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>啥都没写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三次修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次的内容丢失了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -353,17 +365,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
understand what is stage
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdgandzxx\learngit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF40C5E3-B395-4616-9D8D-1DEEE82078C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD70CDA8-EC73-4A99-849D-50573E7AF0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="960" windowWidth="26115" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="960" windowWidth="26115" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>啥都没写</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,6 +40,10 @@
   </si>
   <si>
     <t>第二次的内容丢失了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唉, 找回来了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,30 +369,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>